<commit_message>
improve row comparison add AutomaticallyTrimAllStringValues to excel reader
</commit_message>
<xml_diff>
--- a/Tests/EtLast.Tests.EPPlus/TestData/Sample.xlsx
+++ b/Tests/EtLast.Tests.EPPlus/TestData/Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\EtLast\Tests\EtLast.Tests.EPPlus\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\dev\EtLast\Tests\EtLast.Tests.EPPlus\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CF010B-0B44-47C8-AB3E-AD6AAEDBEE43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30909E50-EE3B-4243-8728-3A2E9CF86025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7C78A9E9-812E-4A2F-84B4-7E0763C07326}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7C78A9E9-812E-4A2F-84B4-7E0763C07326}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t>AAA</t>
-  </si>
-  <si>
     <t>Value1</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>Value4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAA   </t>
   </si>
 </sst>
 </file>
@@ -410,13 +410,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="23.21875" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -424,19 +424,19 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -444,13 +444,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>

</xml_diff>